<commit_message>
Long overdue update including assignments 9 and the start of 10 along with quite a few random scripts I wrote mostly for solving riddlers
</commit_message>
<xml_diff>
--- a/Assignment_1/Runtime Data.xlsx
+++ b/Assignment_1/Runtime Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schultze\Desktop\Learning-Python\Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kschultze\Desktop\Learning-Python\Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7254C4-E7A6-46F0-B827-E6565A6178D0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>rev 2</t>
   </si>
@@ -34,11 +35,14 @@
   <si>
     <t>rev 3.1</t>
   </si>
+  <si>
+    <t>rev 3.1 (C++)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,6 +199,9 @@
                 <c:pt idx="8">
                   <c:v>500000</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -299,6 +306,9 @@
                 <c:pt idx="8">
                   <c:v>500000</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -403,6 +413,9 @@
                 <c:pt idx="8">
                   <c:v>500000</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -438,6 +451,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>68.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,6 +1236,489 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rev 3.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>181</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-957D-43D6-9737-8D5570A8C104}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rev 3.1 (C++)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="6">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.391</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0779999999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.703000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-957D-43D6-9737-8D5570A8C104}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="530145672"/>
+        <c:axId val="530141408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="530145672"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="5000000"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530141408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="530141408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="530145672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1300,6 +1799,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2332,24 +2871,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127635</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>432435</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2366,20 +3427,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>80010</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>384810</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2389,6 +3456,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2EDDA21-3992-462B-A75C-DA0C3E9D62AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2693,16 +3796,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2712,8 +3815,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -2727,7 +3833,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -2741,7 +3847,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5000</v>
       </c>
@@ -2755,7 +3861,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10000</v>
       </c>
@@ -2769,7 +3875,7 @@
         <v>0.26200000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20000</v>
       </c>
@@ -2783,7 +3889,7 @@
         <v>0.71799999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50000</v>
       </c>
@@ -2797,7 +3903,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100000</v>
       </c>
@@ -2810,8 +3916,15 @@
       <c r="D8">
         <v>6.95</v>
       </c>
+      <c r="E8">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F8">
+        <f>D8/E8</f>
+        <v>40.406976744186053</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>200000</v>
       </c>
@@ -2824,8 +3937,15 @@
       <c r="D9">
         <v>18.5</v>
       </c>
+      <c r="E9">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F13" si="0">D9/E9</f>
+        <v>51.532033426183844</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>500000</v>
       </c>
@@ -2837,6 +3957,52 @@
       </c>
       <c r="D10">
         <v>68.099999999999994</v>
+      </c>
+      <c r="E10">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>51.280120481927703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1000000</v>
+      </c>
+      <c r="D11">
+        <v>181</v>
+      </c>
+      <c r="E11">
+        <v>3.391</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>53.37658507814804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2000000</v>
+      </c>
+      <c r="E12">
+        <v>9.0779999999999994</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5000000</v>
+      </c>
+      <c r="E13">
+        <v>33.703000000000003</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>